<commit_message>
buliding out the skeleton structure
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johngraves/Dropbox/teaching/cea-workshop-vital/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6BFB59A6-DC64-C24F-B5F8-04E24A49DF03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D2E0E03-DA85-3140-A90B-65C5A1D390C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="760" windowWidth="34560" windowHeight="19880" activeTab="1" xr2:uid="{AC527668-4C74-614E-AB7C-35A75E6BADEE}"/>
+    <workbookView xWindow="38400" yWindow="760" windowWidth="34560" windowHeight="19880" xr2:uid="{AC527668-4C74-614E-AB7C-35A75E6BADEE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="61">
   <si>
     <t>Day 1</t>
   </si>
@@ -72,9 +72,6 @@
   </si>
   <si>
     <t>Dissemination to policy audiences</t>
-  </si>
-  <si>
-    <t>Case study: Write-up the results of a CEA</t>
   </si>
   <si>
     <t>Capstone: Present model results</t>
@@ -299,6 +296,9 @@
   </si>
   <si>
     <t>Introduction to microsimulation and discrete event simulation modeling</t>
+  </si>
+  <si>
+    <t>Case study: TBD</t>
   </si>
 </sst>
 </file>
@@ -905,7 +905,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF3F9F88-8FB4-1443-9C48-C5E947AE8F5F}">
   <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView zoomScale="158" zoomScaleNormal="158" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="158" zoomScaleNormal="158" workbookViewId="0">
       <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
@@ -930,7 +930,7 @@
         <v>0</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>5</v>
@@ -939,7 +939,7 @@
     <row r="4" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B4" s="31"/>
       <c r="C4" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>10</v>
@@ -948,7 +948,7 @@
     <row r="5" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B5" s="31"/>
       <c r="C5" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>1</v>
@@ -957,7 +957,7 @@
     <row r="6" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B6" s="31"/>
       <c r="C6" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>8</v>
@@ -966,7 +966,7 @@
     <row r="7" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B7" s="31"/>
       <c r="C7" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>6</v>
@@ -975,7 +975,7 @@
     <row r="8" spans="2:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="32"/>
       <c r="C8" s="22" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>9</v>
@@ -986,7 +986,7 @@
         <v>2</v>
       </c>
       <c r="C9" s="21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D9" s="15" t="s">
         <v>7</v>
@@ -995,46 +995,46 @@
     <row r="10" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B10" s="31"/>
       <c r="C10" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B11" s="31"/>
       <c r="C11" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B12" s="31"/>
       <c r="C12" s="12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B13" s="31"/>
       <c r="C13" s="12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B14" s="31"/>
       <c r="C14" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.2">
@@ -1042,93 +1042,93 @@
         <v>3</v>
       </c>
       <c r="C15" s="21" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D15" s="17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B16" s="31"/>
       <c r="C16" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B17" s="31"/>
       <c r="C17" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B18" s="31"/>
       <c r="C18" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B19" s="31"/>
       <c r="C19" s="12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B20" s="32"/>
       <c r="C20" s="22" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D20" s="16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B21" s="30" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C21" s="21" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D21" s="17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B22" s="31"/>
       <c r="C22" s="23" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B23" s="31"/>
       <c r="C23" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="24" spans="2:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="32"/>
       <c r="C24" s="22" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.2">
@@ -1136,7 +1136,7 @@
         <v>4</v>
       </c>
       <c r="C25" s="21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>11</v>
@@ -1145,28 +1145,28 @@
     <row r="26" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B26" s="31"/>
       <c r="C26" s="12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>12</v>
+        <v>60</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B27" s="31"/>
       <c r="C27" s="12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B28" s="32"/>
       <c r="C28" s="22" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.2">
@@ -1174,39 +1174,39 @@
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B30" s="27" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C30" s="18"/>
       <c r="D30" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B31" s="28"/>
       <c r="C31" s="19"/>
       <c r="D31" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B32" s="28"/>
       <c r="C32" s="19"/>
       <c r="D32" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B33" s="28"/>
       <c r="C33" s="19"/>
       <c r="D33" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="34" spans="2:4" ht="34" x14ac:dyDescent="0.2">
       <c r="B34" s="29"/>
       <c r="C34" s="20"/>
       <c r="D34" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -1226,8 +1226,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9445E824-1914-3040-8283-7E0157BEBB4C}">
   <dimension ref="A2:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="149" zoomScaleNormal="149" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView topLeftCell="B1" zoomScale="149" zoomScaleNormal="149" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1244,18 +1244,18 @@
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B2" s="24"/>
       <c r="C2" s="36" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D2" s="34" t="s">
+        <v>57</v>
+      </c>
+      <c r="E2" s="34" t="s">
         <v>58</v>
-      </c>
-      <c r="E2" s="34" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="10" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="25" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C3" s="37"/>
       <c r="D3" s="35"/>
@@ -1296,7 +1296,7 @@
         <v>6</v>
       </c>
       <c r="D6" s="24" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E6" s="24"/>
     </row>
@@ -1319,10 +1319,10 @@
         <v>44790</v>
       </c>
       <c r="C8" s="24" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D8" s="24" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E8" s="24"/>
     </row>
@@ -1332,13 +1332,13 @@
         <v>44797</v>
       </c>
       <c r="C9" s="24" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D9" s="24" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E9" s="24" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -1347,7 +1347,7 @@
         <v>44804</v>
       </c>
       <c r="C10" s="24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D10" s="24"/>
       <c r="E10" s="24"/>
@@ -1358,13 +1358,13 @@
         <v>44811</v>
       </c>
       <c r="C11" s="24" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D11" s="24" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E11" s="24" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -1373,10 +1373,10 @@
         <v>44818</v>
       </c>
       <c r="C12" s="24" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D12" s="24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E12" s="24"/>
     </row>
@@ -1390,7 +1390,7 @@
       </c>
       <c r="D13" s="24"/>
       <c r="E13" s="24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -1399,11 +1399,9 @@
         <v>44832</v>
       </c>
       <c r="C14" s="24" t="s">
-        <v>60</v>
-      </c>
-      <c r="D14" s="24" t="s">
-        <v>12</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="D14" s="24"/>
       <c r="E14" s="24"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>